<commit_message>
updated files from pembina
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/BDbDT/BAU Deaths by Demographic Trait.xlsx
+++ b/InputData/add-outputs/BDbDT/BAU Deaths by Demographic Trait.xlsx
@@ -7591,8 +7591,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010010EB76B7FE121F489C7B2A4727FCE3E9" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fdee17017a9ad5b872047a216f95da93">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="52604411-7aeb-406e-8b34-4ce79a7293cc" xmlns:ns3="de340059-046a-4f1a-8b62-ade039df3700" xmlns:ns4="d580559a-617d-4d7d-8fb9-71ff64b58360" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="37825e9edfcb807d863c63152c6d8635" ns2:_="" ns3:_="" ns4:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010010EB76B7FE121F489C7B2A4727FCE3E9" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b14dc5c440242a7f7d08dacad5c84df8">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="52604411-7aeb-406e-8b34-4ce79a7293cc" xmlns:ns3="de340059-046a-4f1a-8b62-ade039df3700" xmlns:ns4="d580559a-617d-4d7d-8fb9-71ff64b58360" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71a713f9ca42e4f2f02aa83a9b465f65" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="52604411-7aeb-406e-8b34-4ce79a7293cc"/>
     <xsd:import namespace="de340059-046a-4f1a-8b62-ade039df3700"/>
     <xsd:import namespace="d580559a-617d-4d7d-8fb9-71ff64b58360"/>
@@ -7618,6 +7618,7 @@
                 <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -7718,6 +7719,11 @@
     <xsd:element name="MediaServiceDateTaken" ma:index="27" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="28" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -7859,5 +7865,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51754610-9DEC-4D71-AB5E-7F6C384D251C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC24D3D0-CC8B-4FE2-AB77-F57AA25DC568}"/>
 </file>
</xml_diff>